<commit_message>
Export to .xlsx successfully
</commit_message>
<xml_diff>
--- a/bin/Debug/net8.0-windows/reports/userlist.xlsx
+++ b/bin/Debug/net8.0-windows/reports/userlist.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,18 +19,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>username</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>admin</t>
   </si>
   <si>
     <t>password</t>
   </si>
   <si>
-    <t>email</t>
+    <t>Shakira Regalado</t>
+  </si>
+  <si>
+    <t>shakiraregalado@gmail.com</t>
+  </si>
+  <si>
+    <t>Fluffy</t>
+  </si>
+  <si>
+    <t>kira</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Shakira</t>
+  </si>
+  <si>
+    <t>shakira@gmail.com</t>
+  </si>
+  <si>
+    <t>Pink</t>
   </si>
 </sst>
 </file>
@@ -348,26 +366,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D2"/>
+  <dimension ref="A2:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify home page and export directory, and add installer
</commit_message>
<xml_diff>
--- a/bin/Debug/net8.0-windows/reports/userlist.xlsx
+++ b/bin/Debug/net8.0-windows/reports/userlist.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Security Question</t>
+  </si>
+  <si>
+    <t>Security Answer</t>
+  </si>
   <si>
     <t>admin</t>
   </si>
@@ -366,33 +387,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -400,22 +451,22 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F3">
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>